<commit_message>
Interface elements (Actions, Skill Usage, NumberSpawner impruvment) and Fire Skill Test
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE12BC7-4D95-466E-B5D0-6E05531A0DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2677C95A-2FD8-4058-86BD-497DB5BB320B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>CoolDown</t>
+  </si>
+  <si>
+    <t>FieryFlicker</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,6 +487,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
All elemental abilities tests (Water, Plant, Earth, Wind, Thunder, Light and Darknes)
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2677C95A-2FD8-4058-86BD-497DB5BB320B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082813AF-8E07-4457-8F78-867B7EFAE08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -52,6 +52,27 @@
   </si>
   <si>
     <t>FieryFlicker</t>
+  </si>
+  <si>
+    <t>DoubleDelta</t>
+  </si>
+  <si>
+    <t>RockyRumble</t>
+  </si>
+  <si>
+    <t>ThornyThrust</t>
+  </si>
+  <si>
+    <t>ChargedContact</t>
+  </si>
+  <si>
+    <t>GulibleGust</t>
+  </si>
+  <si>
+    <t>LuminousLash</t>
+  </si>
+  <si>
+    <t>ShadowSlice</t>
   </si>
 </sst>
 </file>
@@ -420,16 +441,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="2"/>
     <col min="5" max="5" width="10.140625" style="2" bestFit="1" customWidth="1"/>
@@ -504,6 +525,125 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cure, Healing and OnHealing Trigger Sweep Test (Sucess)
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082813AF-8E07-4457-8F78-867B7EFAE08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F87B659-EAF5-40FA-962E-91F4A10B758A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>ShadowSlice</t>
+  </si>
+  <si>
+    <t>CureI</t>
+  </si>
+  <si>
+    <t>StatusSkill</t>
   </si>
 </sst>
 </file>
@@ -441,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,6 +650,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Passive Skills and Passive Skills Logic
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F87B659-EAF5-40FA-962E-91F4A10B758A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5B132F-C8B4-4C43-93DA-2DACCA7D738F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -79,13 +79,19 @@
   </si>
   <si>
     <t>StatusSkill</t>
+  </si>
+  <si>
+    <t>EmergencySupplies</t>
+  </si>
+  <si>
+    <t>PassiveSkill</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +116,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,7 +167,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -162,6 +176,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -447,23 +464,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="2"/>
     <col min="5" max="5" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,7 +497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -497,7 +514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -514,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -531,7 +548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -548,7 +565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -565,7 +582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -582,7 +599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -599,7 +616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -616,7 +633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -633,7 +650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -650,7 +667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -666,8 +683,32 @@
       <c r="E12" s="3">
         <v>3</v>
       </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reflect BUFF and Receive Damage context Triggers
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5B132F-C8B4-4C43-93DA-2DACCA7D738F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED7188D-1D09-4015-B38B-4A9110D700C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>PassiveSkill</t>
+  </si>
+  <si>
+    <t>ScaleOneself</t>
   </si>
 </sst>
 </file>
@@ -467,7 +470,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,9 +705,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="3">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Haste Status and TurnStart trigger context test
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED7188D-1D09-4015-B38B-4A9110D700C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499DF77F-505E-4540-AA04-FF4064782593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -88,13 +88,16 @@
   </si>
   <si>
     <t>ScaleOneself</t>
+  </si>
+  <si>
+    <t>LimiterRemoval</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +130,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,7 +181,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -182,6 +193,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -467,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,6 +736,26 @@
         <v>3</v>
       </c>
     </row>
+    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="3">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
onGotTargeted context trigger Logic + 1 Passive Skill (Force of Habit)
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499DF77F-505E-4540-AA04-FF4064782593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192B0D6B-64CF-4433-B0EC-DEF622B054BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -91,13 +91,16 @@
   </si>
   <si>
     <t>LimiterRemoval</t>
+  </si>
+  <si>
+    <t>ForceOfHabit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,14 +133,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,7 +176,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -193,9 +188,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -484,7 +476,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,8 +745,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F16" s="5"/>
+    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Has Effect Logic in Damage Skill. Content Spawner with InAction/OutAction. onDamageCalc context test and Exhaust Status Effect
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192B0D6B-64CF-4433-B0EC-DEF622B054BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A238283-36B5-43EA-85E3-45D08E3FD1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>ForceOfHabit</t>
+  </si>
+  <si>
+    <t>OpressTheWeak</t>
+  </si>
+  <si>
+    <t>DamageSkill(has effect)</t>
   </si>
 </sst>
 </file>
@@ -473,17 +479,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="2"/>
     <col min="5" max="5" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="2"/>
@@ -762,6 +768,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="3">
+        <v>20</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
OnCriticalCalc Trigger context test + Focus Status Effect
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A238283-36B5-43EA-85E3-45D08E3FD1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4D9200-7ADA-4817-B302-079738CC2E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>DamageSkill(has effect)</t>
+  </si>
+  <si>
+    <t>TrueVision</t>
   </si>
 </sst>
 </file>
@@ -479,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,6 +788,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3">
+        <v>13</v>
+      </c>
+      <c r="E18" s="3">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Blind Status + onAccuracyCalc Trigger context test
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4D9200-7ADA-4817-B302-079738CC2E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E829EACF-24BF-4A1D-BF6B-6E7D6A966322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>TrueVision</t>
+  </si>
+  <si>
+    <t>WillfullIgnorance</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,6 +808,23 @@
         <v>7</v>
       </c>
     </row>
+    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="3">
+        <v>15</v>
+      </c>
+      <c r="E19" s="3">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Precision Status + onGetStatus trigger context test
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E829EACF-24BF-4A1D-BF6B-6E7D6A966322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FF0181-6F01-4DDA-9CDC-C638B1E78F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>WillfullIgnorance</t>
+  </si>
+  <si>
+    <t>NaturalLens</t>
   </si>
 </sst>
 </file>
@@ -485,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,6 +828,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Poison Status Effect + OnTurnEnd Trigger context bug fix
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FF0181-6F01-4DDA-9CDC-C638B1E78F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978A94D1-F64F-4527-9E39-A8DB0B678A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>NaturalLens</t>
+  </si>
+  <si>
+    <t>EfficientCasting</t>
+  </si>
+  <si>
+    <t>PoisonMaw</t>
   </si>
 </sst>
 </file>
@@ -488,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,21 +834,55 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="2">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0</v>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3">
+        <v>10</v>
+      </c>
+      <c r="E22" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OnPassingTurn Trigger context + OnTurnEnd context logic change
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978A94D1-F64F-4527-9E39-A8DB0B678A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6AC1A5-41A5-4725-8A53-75BEAEAA5C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>PoisonMaw</t>
+  </si>
+  <si>
+    <t>SlowAntibodies</t>
   </si>
 </sst>
 </file>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,6 +888,23 @@
         <v>3</v>
       </c>
     </row>
+    <row r="23" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Slow Status Effect + OnGettingActions Trigger context + Show Number timer add
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6AC1A5-41A5-4725-8A53-75BEAEAA5C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80FAF42-D943-4036-AA8B-C6525BAA7FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>SlowAntibodies</t>
+  </si>
+  <si>
+    <t>LimiterOverload</t>
   </si>
 </sst>
 </file>
@@ -497,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,6 +908,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="24" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="3">
+        <v>9</v>
+      </c>
+      <c r="E24" s="3">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Barrier Status Effect + getHited Trigger Context Logic change.
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80FAF42-D943-4036-AA8B-C6525BAA7FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F2D6EF-783A-4F00-9B9F-9C415F9DB8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>LimiterOverload</t>
+  </si>
+  <si>
+    <t>DimensionalBarrier</t>
   </si>
 </sst>
 </file>
@@ -500,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,6 +928,23 @@
         <v>3</v>
       </c>
     </row>
+    <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="3">
+        <v>12</v>
+      </c>
+      <c r="E25" s="3">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
OnEvadeDamage trigger context test + Mark Status Effect
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F2D6EF-783A-4F00-9B9F-9C415F9DB8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7BF284-67FC-4686-873A-91922DB8F11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>DimensionalBarrier</t>
+  </si>
+  <si>
+    <t>InstinctiveEvasion</t>
+  </si>
+  <si>
+    <t>MarkingDodge</t>
   </si>
 </sst>
 </file>
@@ -503,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,6 +951,40 @@
         <v>7</v>
       </c>
     </row>
+    <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
OnEvadeStatus trigger context test
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7BF284-67FC-4686-873A-91922DB8F11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F155371-6917-49C5-8BB6-29FB4E2AC59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>MarkingDodge</t>
+  </si>
+  <si>
+    <t>CounterMagic</t>
   </si>
 </sst>
 </file>
@@ -509,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,6 +988,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Animation Queue System + onUnapplyingStatus trigger context test + Unstoppable Status Effect
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F155371-6917-49C5-8BB6-29FB4E2AC59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5780A28E-3FF9-4C30-9E7C-84F5DEE09097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>CounterMagic</t>
+  </si>
+  <si>
+    <t>WindsOverTheIceBarrier</t>
+  </si>
+  <si>
+    <t>AGlacialHeart</t>
   </si>
 </sst>
 </file>
@@ -512,16 +518,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="2"/>
     <col min="5" max="5" width="10.140625" style="2" bestFit="1" customWidth="1"/>
@@ -1005,6 +1011,40 @@
         <v>0</v>
       </c>
     </row>
+    <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="3">
+        <v>8</v>
+      </c>
+      <c r="E29" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
OnActing trigger context text
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5780A28E-3FF9-4C30-9E7C-84F5DEE09097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F922FD51-1529-4E14-BACF-431F6494A274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>AGlacialHeart</t>
+  </si>
+  <si>
+    <t>BackupStrike</t>
   </si>
 </sst>
 </file>
@@ -518,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,6 +1048,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>29</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3">
+        <v>5</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
INTPLUS and INTMINUS status effect + Attributes card on digimonDisplay
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F922FD51-1529-4E14-BACF-431F6494A274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DBF7E3-CE77-4DE8-9EC3-36DD8BDD1FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>BackupStrike</t>
+  </si>
+  <si>
+    <t>Counting</t>
   </si>
 </sst>
 </file>
@@ -521,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,6 +1068,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="32" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Campaign Global class as Reference + procedural teste generator
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B320DC5-3A88-4EA2-98B7-AD8399DB4E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E189E7-0E48-4677-83DB-FF1310DFDB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>BluntAttack</t>
+  </si>
+  <si>
+    <t>SupplySquad</t>
   </si>
 </sst>
 </file>
@@ -541,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,8 +1171,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+    <row r="37" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>35</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
OnChnaging triggers context test
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8619533-BCB8-4720-BB17-D3A9467C9C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6554E0D-27DE-4100-B117-C77B665C2432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>DamageSkill(Betamon)</t>
+  </si>
+  <si>
+    <t>AvengerPact</t>
+  </si>
+  <si>
+    <t>PassiveSkill(Monodramon)</t>
   </si>
 </sst>
 </file>
@@ -608,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,6 +1447,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="49" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>47</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Enemy evolution and digimon exchange
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC41576-3C5B-414D-A742-1FB97D758A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08738C4E-DD0F-4F81-B273-1CDE288E6A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="104">
   <si>
     <t>ID</t>
   </si>
@@ -334,13 +334,16 @@
   </si>
   <si>
     <t>DamageSkill(Stingmon)</t>
+  </si>
+  <si>
+    <t>SurvivalBaton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,6 +376,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -416,7 +427,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -428,6 +439,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -713,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,6 +1866,26 @@
         <v>4</v>
       </c>
     </row>
+    <row r="67" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>65</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D67" s="3">
+        <v>0</v>
+      </c>
+      <c r="E67" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bug fix (Confirmation fade vanishing, windows forced close and button panel conflit) and Interface update on language change.
</commit_message>
<xml_diff>
--- a/documentation/SkillsDatabase.xlsx
+++ b/documentation/SkillsDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF3A6EC-475F-47CE-894B-9730E9C82C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715A27B6-98DE-4FB2-99C9-F8C8F4A8B943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -729,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>